<commit_message>
Se agrega campo supervisor_asignado en registro de asistencia_persona'
</commit_message>
<xml_diff>
--- a/data/data_prueba.xlsx
+++ b/data/data_prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskar\Documents\Proto\Learning\php\registro_tiempo_vainilla\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\registro-asistencia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C35484C-49CA-413E-970A-2A1F4BACEF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110A848E-8F37-4424-A6E1-73F49A3A2AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{49ED3FA5-E3E2-4AF5-B3CF-82337236FE2D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Apellido</t>
   </si>
@@ -105,13 +105,22 @@
   </si>
   <si>
     <t>Query Insert</t>
+  </si>
+  <si>
+    <t>pedro</t>
+  </si>
+  <si>
+    <t>perez</t>
+  </si>
+  <si>
+    <t>pedro.perez@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +143,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,8 +169,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -161,9 +179,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -180,22 +199,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -267,6 +270,22 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -281,14 +300,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85DC2BA4-F096-4108-ADC7-39F5AB04DC31}" name="Table1" displayName="Table1" ref="A3:E9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A3:E9" xr:uid="{85DC2BA4-F096-4108-ADC7-39F5AB04DC31}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85DC2BA4-F096-4108-ADC7-39F5AB04DC31}" name="Table1" displayName="Table1" ref="A3:E10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E10" xr:uid="{85DC2BA4-F096-4108-ADC7-39F5AB04DC31}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0319444E-7700-45AB-BABA-B9C694184F15}" name="DNI" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{31583143-87B9-447F-A1AF-28EFB00AE331}" name=" Nombre" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{1B58C302-BD3F-4DCD-9FC3-9D7EFD743D16}" name="Apellido" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{D2FF00E3-A294-48E5-BB62-A6624D90AB4F}" name="email" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{02B8B677-D3D9-4737-A8B0-191B809EDCA0}" name="Query Insert" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{0319444E-7700-45AB-BABA-B9C694184F15}" name="DNI" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{31583143-87B9-447F-A1AF-28EFB00AE331}" name=" Nombre" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{1B58C302-BD3F-4DCD-9FC3-9D7EFD743D16}" name="Apellido" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D2FF00E3-A294-48E5-BB62-A6624D90AB4F}" name="email" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{02B8B677-D3D9-4737-A8B0-191B809EDCA0}" name="Query Insert" dataDxfId="0">
       <calculatedColumnFormula>"INSERT INTO `persona` (`dni`,`nombre`,`apellido`,`email`) VALUES ('" &amp; A4 &amp; "', '" &amp; B4 &amp; "', '" &amp; C4 &amp; "', '" &amp; D4 &amp; "' );"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -613,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC736163-E9C2-4DF1-A325-F4932A5A441E}">
-  <dimension ref="A3:E9"/>
+  <dimension ref="A3:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +674,7 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2" t="str">
@@ -673,7 +692,7 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="2" t="str">
@@ -691,7 +710,7 @@
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="2" t="str">
@@ -709,7 +728,7 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="2" t="str">
@@ -727,7 +746,7 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="2" t="str">
@@ -745,7 +764,7 @@
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2" t="str">
@@ -753,11 +772,32 @@
         <v>INSERT INTO `persona` (`dni`,`nombre`,`apellido`,`email`) VALUES ('79975554', 'Leonardo Pedro', 'Carpio Jimenez', 'leonardo.carpio@gmail.com' );</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f>"INSERT INTO `persona` (`dni`,`nombre`,`apellido`,`email`) VALUES ('" &amp; A10 &amp; "', '" &amp; B10 &amp; "', '" &amp; C10 &amp; "', '" &amp; D10 &amp; "' );"</f>
+        <v>INSERT INTO `persona` (`dni`,`nombre`,`apellido`,`email`) VALUES ('99', 'pedro', 'perez', 'pedro.perez@gmail.com' );</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{2F861D81-6CEC-462F-9641-3710B101D2D2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>